<commit_message>
screenshot &cocumber and step definitions updated
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/testdata.xlsx
+++ b/src/main/java/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ROMEDA\sprint-workspace\AsianPaints_LoginPage_Rohith\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4FBC01-F7AC-4BAE-91EC-443D65ACBCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2ECF925-AF05-453B-A96A-7A5E1620ACB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>